<commit_message>
Descargar CSV resultante de RFE
</commit_message>
<xml_diff>
--- a/sistemaaid/variablesSeleccionadasPorRFE3.xlsx
+++ b/sistemaaid/variablesSeleccionadasPorRFE3.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.02453126129108428</v>
+        <v>0.02133739055988834</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.002708759908471674</v>
+        <v>0.002626244732546388</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.001566843873912228</v>
+        <v>0.001722929952235951</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.007627281350997487</v>
+        <v>0.008900567740567158</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01538699478106809</v>
+        <v>0.0126293398289155</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.007073993330031057</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.004175376976497221</v>
+        <v>0.004105961597367491</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.003713831019783253</v>
+        <v>0.005038064068339945</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.004789519387825843</v>
+        <v>0.004614606972639613</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.004439366205410762</v>
+        <v>0.00414569718658213</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.003794875685210469</v>
+        <v>0.00202729292261339</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.00495438394839759</v>
+        <v>0.005126615303277494</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.004001931239801638</v>
+        <v>0.004041235218729556</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.003525421566044425</v>
+        <v>0.003665028351699451</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.005866310533801116</v>
+        <v>0.005465355404752728</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.004528903983919458</v>
+        <v>0.004995587691683621</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.003424290305463388</v>
+        <v>0.003785244935130975</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.004608108865662711</v>
+        <v>0.00473401263742543</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.002872911263852662</v>
+        <v>0.002348337830784448</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.01171386309441066</v>
+        <v>0.01555413382075052</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.003417395986222034</v>
+        <v>0.003172742102786743</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.002345881967473687</v>
+        <v>0.002611694663865061</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.00181765647716779</v>
+        <v>0.001694278457347614</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.01003508242700205</v>
+        <v>0.01743563644069842</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.00238186358447124</v>
+        <v>0.002162332697110018</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.002693688311532333</v>
+        <v>0.002653774029066915</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.002354911299007259</v>
+        <v>0.001927700122934736</v>
       </c>
     </row>
     <row r="29">
@@ -722,577 +722,577 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.002059963904587377</v>
+        <v>0.002218947647459677</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>P22_Suponiendo que las universidades de tu agrado inicien estudios PRESENCIALES en septiembre de 2020, ¿qué tan probable es que inicies una carrera larga?</t>
+          <t>P21_Suponiendo que las universidades de tu agrado inicien estudios EN LÍNEA en septiembre de 2020, ¿qué tan probable es que inicies una carrera larga?</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.01204893518557788</v>
+        <v>0.003486445953284074</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>P23_Suponiendo que las universidades de tu agrado inicien estudios MIXTO (presencial y en línea) en septiembre de 2020, ¿qué tan probable es que inicies una carrera larga?</t>
+          <t>P22_Suponiendo que las universidades de tu agrado inicien estudios PRESENCIALES en septiembre de 2020, ¿qué tan probable es que inicies una carrera larga?</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.00594092178321675</v>
+        <v>0.0117025467639095</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>P24_Pensando en los planes que tenías antes de comenzar la pandemia, ¿qué crees que harás llegado septiembre de 2020?</t>
+          <t>P23_Suponiendo que las universidades de tu agrado inicien estudios MIXTO (presencial y en línea) en septiembre de 2020, ¿qué tan probable es que inicies una carrera larga?</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.01834332319665325</v>
+        <v>0.01780945951377177</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>P25_CODIF_¿Qué opinan tus padres de cara a realizar estudios superiores en septiembre del 2020, considerando la pandemia COVID -19?</t>
+          <t>P24_Pensando en los planes que tenías antes de comenzar la pandemia, ¿qué crees que harás llegado septiembre de 2020?</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.02123498926636951</v>
+        <v>0.01188801892300044</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>P.10_¿Tienes_algun_familiar_o_conocido_cercano_de_la_UCAB?</t>
+          <t>P25_CODIF_¿Qué opinan tus padres de cara a realizar estudios superiores en septiembre del 2020, considerando la pandemia COVID -19?</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.002357154525008807</v>
+        <v>0.01591051405519939</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>P.2A1_primeras_tres_opciones_de_carrera_CODIF_1</t>
+          <t>P.10_¿Tienes_algun_familiar_o_conocido_cercano_de_la_UCAB?</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.008210033609321574</v>
+        <v>0.002810608681229709</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>P1RA_univ_CODIF_1</t>
+          <t>P.2A1_primeras_tres_opciones_de_carrera_CODIF_1</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.01926670745608581</v>
+        <v>0.008413618899918419</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>P2DA_univ_CODIF_1</t>
+          <t>P1RA_univ_CODIF_1</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.002414574103805604</v>
+        <v>0.01592436552818343</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>P3RA_univ_CODIF_1</t>
+          <t>P2DA_univ_CODIF_1</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.002940587070161199</v>
+        <v>0.00317054598159212</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>P.2A2_primeras_tres_opciones_de_carrera_CODIF_2</t>
+          <t>P3RA_univ_CODIF_1</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.007725891095538734</v>
+        <v>0.003308886810992527</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>P1RA_univ_CODIF_2</t>
+          <t>P.2A2_primeras_tres_opciones_de_carrera_CODIF_2</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.004095699979477123</v>
+        <v>0.008471451889248199</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>P2DA_univ_CODIF_2</t>
+          <t>P1RA_univ_CODIF_2</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.001465148087321606</v>
+        <v>0.003616807248764491</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>P.2A3_primeras_tres_opciones_de_carrera_CODIF_3</t>
+          <t>P2DA_univ_CODIF_2</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.006583536321382883</v>
+        <v>0.00136902309623599</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>P1RA_univ_CODIF_3</t>
+          <t>P.2A3_primeras_tres_opciones_de_carrera_CODIF_3</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.00350101498161601</v>
+        <v>0.006753926128423295</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>P2DA_univ_CODIF_3</t>
+          <t>P1RA_univ_CODIF_3</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.001220760627011301</v>
+        <v>0.003159792672603116</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>P.2C_¿Por_qué_es_esa_tu_primera_opción_de_carrera?_CODIF_1</t>
+          <t>P2DA_univ_CODIF_3</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.00393228568214089</v>
+        <v>0.001400509208782498</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>P.2D_¿Por_qué_es_esa_tu_primera_opción_de_Universidad_para_estudiar_esa_carrera?_CODIF_1</t>
+          <t>P.2C_¿Por_qué_es_esa_tu_primera_opción_de_carrera?_CODIF_1</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.006894903061754821</v>
+        <v>0.003578720140227159</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>P.2E_¿Qué_tan_seguro(a)_te_sientes_sobre_tu_primera_opción_de_carrera?</t>
+          <t>P.2D_¿Por_qué_es_esa_tu_primera_opción_de_Universidad_para_estudiar_esa_carrera?_CODIF_1</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.01019162867542596</v>
+        <v>0.006572461338962517</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>P.2F_¿Cuál_carrera_jamás_estudiarías_aunque_tuvieras_la_oportunidad?_CODIF</t>
+          <t>P.2E_¿Qué_tan_seguro(a)_te_sientes_sobre_tu_primera_opción_de_carrera?</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.005537278076706778</v>
+        <v>0.01531148038242812</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>P.2G_¿Por_qué_esa_carrera?_CODIF</t>
+          <t>P.2F_¿Cuál_carrera_jamás_estudiarías_aunque_tuvieras_la_oportunidad?_CODIF</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.001636334772193902</v>
+        <v>0.005642688157678928</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>P.2H_¿En_cuál_universidad_jamás_estudiarías_aunque_tuvieras_la_oportunidad?_CODIF</t>
+          <t>P.2G_¿Por_qué_esa_carrera?_CODIF</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.003077031074072335</v>
+        <v>0.002141551212283954</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>P3_Calificación_General_UCV</t>
+          <t>P.2H_¿En_cuál_universidad_jamás_estudiarías_aunque_tuvieras_la_oportunidad?_CODIF</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.00588755091732771</v>
+        <v>0.003102879415812946</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>P3._Calificación_General_UNIMET</t>
+          <t>P3_Calificación_General_UCV</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.004976713430479417</v>
+        <v>0.005160687688269135</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>P3._Calificación_General_USB</t>
+          <t>P3._Calificación_General_UNIMET</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.005041276986138069</v>
+        <v>0.005358347633982311</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>P3._Calificación_General_USM</t>
+          <t>P3._Calificación_General_USB</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.005585034085935046</v>
+        <v>0.004786067604796184</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>P3._Calificación_General_UCAB</t>
+          <t>P3._Calificación_General_USM</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.005754800220917149</v>
+        <v>0.005363651847848355</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>P3._Calificación_General_UMA</t>
+          <t>P3._Calificación_General_UCAB</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.004694380419381001</v>
+        <v>0.005417684501223524</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>P.4_¿De_qué_dependen_en_mayor_medida_las_oportunidades_laborales_de_un_profesional?</t>
+          <t>P3._Calificación_General_UMA</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.003060603637256475</v>
+        <v>0.005108363492957163</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>P.6A_¿Cuán_importantes_son_para_ti_los_conflictos_y_paros_de_las_universidades_públicas_en_tu_decisión_de_estudiar_o_no_en_una_universidad privada?</t>
+          <t>P.4_¿De_qué_dependen_en_mayor_medida_las_oportunidades_laborales_de_un_profesional?</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.01785114136852388</v>
+        <v>0.003119926618289008</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>P.7AE_Son_las_universidades_donde_ya_me_preinscribí_o_me_pienso_preinscribir_UCAB</t>
+          <t>P.6A_¿Cuán_importantes_son_para_ti_los_conflictos_y_paros_de_las_universidades_públicas_en_tu_decisión_de_estudiar_o_no_en_una_universidad privada?</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.004608436079281961</v>
+        <v>0.004295747908697487</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>P.7AE_Son_las_universidades_donde_ya_me_preinscribí_o_me_pienso_preinscribir_UCV</t>
+          <t>P.7AE_Son_las_universidades_donde_ya_me_preinscribí_o_me_pienso_preinscribir_UCAB</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.001148971860180733</v>
+        <v>0.005510656604940143</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>P.7A_Tienen_buenas_instalaciones_y_recursos._UCAB</t>
+          <t>P.7AE_Son_las_universidades_donde_ya_me_preinscribí_o_me_pienso_preinscribir_UCV</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.001617543465589294</v>
+        <v>0.001445596592704624</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>P.7A_Tienen_buenas_instalaciones_y_recursos_UNIMET</t>
+          <t>P.7A_Tienen_buenas_instalaciones_y_recursos._UCAB</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.001735644788837399</v>
+        <v>0.003748251504793964</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>P.7A_Tienen_buenas_instalaciones_y_recursos_USB</t>
+          <t>P.7A_Tienen_buenas_instalaciones_y_recursos_UNIMET</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.001261578064572125</v>
+        <v>0.001448739671844033</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>P.7A_Tienen_buenas_instalaciones_y_recursos_UMA</t>
+          <t>P.7A_Tienen_buenas_instalaciones_y_recursos_USM</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.001194636540846108</v>
+        <v>0.00111693949764969</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>P.7A_Tienen_buenas_instalaciones_y_recursos_UCV</t>
+          <t>P.7A_Tienen_buenas_instalaciones_y_recursos_USB</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.001700793164764772</v>
+        <v>0.001332259981325879</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>P.7B_Tienen_prestigio. UCAB</t>
+          <t>P.7A_Tienen_buenas_instalaciones_y_recursos_UMA</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.001442956193617807</v>
+        <v>0.001140766043770062</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>P.7B_Tienen_prestigio. UNIMET</t>
+          <t>P.7A_Tienen_buenas_instalaciones_y_recursos_UCV</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.00166924918119293</v>
+        <v>0.001825946205858712</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>P.7B_Tienen_prestigio. USM</t>
+          <t>P.7B_Tienen_prestigio. UCAB</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.001260831835766435</v>
+        <v>0.001769967625491659</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>P.7B_Tienen_prestigio. USB</t>
+          <t>P.7B_Tienen_prestigio. UNIMET</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.001454107283924962</v>
+        <v>0.001361435467945452</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>P.7B_Tienen_prestigio. UCV</t>
+          <t>P.7B_Tienen_prestigio. USB</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.001217800167867925</v>
+        <v>0.001584681209504945</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>P.7C_Son_costosas. UCAB</t>
+          <t>P.7B_Tienen_prestigio. UMA</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.001293610324566063</v>
+        <v>0.0008497683989763779</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>P.7C_Son_costosas. UNIMET</t>
+          <t>P.7B_Tienen_prestigio. UCV</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.001467193688071433</v>
+        <v>0.00122247445648154</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>P.7C_Son_costosas. USM</t>
+          <t>P.7C_Son_costosas. UCAB</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.001129995239253958</v>
+        <v>0.001399700141217561</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>P.7C_Son_costosas. UMA</t>
+          <t>P.7C_Son_costosas. UNIMET</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.001217230148894117</v>
+        <v>0.001388953427915484</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>P.7D_Ofrecen_variedad_de_carreras_de_pregrado. UCAB</t>
+          <t>P.7C_Son_costosas. USM</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.001840055927424185</v>
+        <v>0.001253541870317971</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>P.7D_Ofrecen_variedad_de_carreras_de_pregrado. UNIMET</t>
+          <t>P.7C_Son_costosas. UMA</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.001257962876481177</v>
+        <v>0.001464383191173976</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>P.7D_Ofrecen_variedad_de_carreras_de_pregrado. USB</t>
+          <t>P.7D_Ofrecen_variedad_de_carreras_de_pregrado. UCAB</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.001035580783650305</v>
+        <v>0.001329823549613837</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>P.7D_Ofrecen_variedad_de_carreras_de_pregrado. UCV</t>
+          <t>P.7D_Ofrecen_variedad_de_carreras_de_pregrado. USB</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.001365037966487643</v>
+        <v>0.001296955054339048</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>P.7E_Tienen_profesores_con_buena_formación_y_nivel.UCAB</t>
+          <t>P.7D_Ofrecen_variedad_de_carreras_de_pregrado. UCV</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.001384040262958569</v>
+        <v>0.001490486281392338</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>P.7E_Tienen_profesores_con_buena_formación_y_nivel.UNIMET</t>
+          <t>P.7E_Tienen_profesores_con_buena_formación_y_nivel.UCAB</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.001385626594211392</v>
+        <v>0.001449882555035126</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>P.7E_Tienen_profesores_con_buena_formación_y_nivel.USM</t>
+          <t>P.7E_Tienen_profesores_con_buena_formación_y_nivel.UNIMET</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.0009779587059474217</v>
+        <v>0.001122521585680538</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>P.7E_Tienen_profesores_con_buena_formación_y_nivel.USB</t>
+          <t>P.7E_Tienen_profesores_con_buena_formación_y_nivel.USM</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.001370024164489202</v>
+        <v>0.0008755216755461016</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>P.7E_Tienen_profesores_con_buena_formación_y_nivel.UCV</t>
+          <t>P.7E_Tienen_profesores_con_buena_formación_y_nivel.USB</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.001753856331299564</v>
+        <v>0.0009981379456695662</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>P.BX_Son_las_mejores_para_las_carreras_de_administración UCAB</t>
+          <t>P.7E_Tienen_profesores_con_buena_formación_y_nivel.UCV</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.0009675572297556093</v>
+        <v>0.001846924289621774</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>P.7F_Ofrecen_más_seguridad_dentro_de_sus_instalaciones UCAB</t>
+          <t>P.BX_Son_las_mejores_para_las_carreras_de_administración UCAB</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.001278858080144403</v>
+        <v>0.001022321486043541</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>P.7G_Hay_que_pagar_sobornos_o_favores_para_pasar_materias. USM</t>
+          <t>P.7F_Ofrecen_más_seguridad_dentro_de_sus_instalaciones UCAB</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.0009238118226857191</v>
+        <v>0.001000558700413936</v>
       </c>
     </row>
     <row r="87">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.001905579913291728</v>
+        <v>0.001513133328352916</v>
       </c>
     </row>
     <row r="88">
@@ -1312,697 +1312,697 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.0009548365233679705</v>
+        <v>0.001446547301994696</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>P.7I_Tienen_alta_exigencia_académica. USB</t>
+          <t>P.7I_Tienen_alta_exigencia_académica. UCV</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.002207918119035998</v>
+        <v>0.001265265237429196</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>P.7I_Tienen_alta_exigencia_académica. UMA</t>
+          <t>P.7J_Tienen_buena_organización_administrativa. UCAB</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.001298167172680792</v>
+        <v>0.002457794778913763</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>P.7I_Tienen_alta_exigencia_académica. UCV</t>
+          <t>P.7J_Tienen_buena_organización_administrativa. UNIMET</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.001151687075305608</v>
+        <v>0.001350466196322328</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>P.7J_Tienen_buena_organización_administrativa. UCAB</t>
+          <t>P.7J_Tienen_buena_organización_administrativa. USB</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.004138187127672235</v>
+        <v>0.001370258758154917</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>P.7J_Tienen_buena_organización_administrativa. UNIMET</t>
+          <t>P.7K_Ofrecen_las_carreras_demandadas_laboralmente UCAB</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.001650938322517301</v>
+        <v>0.001811236004178544</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>P.7J_Tienen_buena_organización_administrativa. USB</t>
+          <t>P.7K_Ofrecen_las_carreras_demandadas_laboralmente UNIMET</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.001117124745925851</v>
+        <v>0.00108786330916985</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>P.7J_Tienen_buena_organización_administrativa. UCV</t>
+          <t>P.7K_Ofrecen_las_carreras_demandadas_laboralmente USM</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.00142867112368404</v>
+        <v>0.0008901170898616223</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>P.7K_Ofrecen_las_carreras_demandadas_laboralmente UCAB</t>
+          <t>P.7K_Ofrecen_las_carreras_demandadas_laboralmente USB</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.001858881905849482</v>
+        <v>0.001321578925466036</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>P.7K_Ofrecen_las_carreras_demandadas_laboralmente UNIMET</t>
+          <t>P.7K_Ofrecen_las_carreras_demandadas_laboralmente UCV</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.001008886274246144</v>
+        <v>0.001250943428243686</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>P.7K_Ofrecen_las_carreras_demandadas_laboralmente UCV</t>
+          <t>P.7M_Están_politizadas USB</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0.001311009056323517</v>
+        <v>0.0009272542852210879</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>P.7M_Están_politizadas USB</t>
+          <t>P.7M_Están_politizadas UCV</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.001323462486323458</v>
+        <v>0.00119666997368019</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>P.7M_Están_politizadas UCV</t>
+          <t>P.7BE_Está_lejos_en_distancia UCAB</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.001054260557708021</v>
+        <v>0.00129321881526101</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>P.7BE_Está_lejos_en_distancia UCAB</t>
+          <t>P.7BE_Está_lejos_en_distancia UNIMET</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.001207358109451828</v>
+        <v>0.001619066054659566</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>P.7BE_Está_lejos_en_distancia UNIMET</t>
+          <t>P.7BE_Está_lejos_en_distancia USM</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.001195714112691991</v>
+        <v>0.001306492674431809</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>P.7BE_Está_lejos_en_distancia USM</t>
+          <t>P.7BE_Está_lejos_en_distancia USB</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.001515509777520062</v>
+        <v>0.001472584789449845</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>P.7BE_Está_lejos_en_distancia USB</t>
+          <t>P.7BE_Está_lejos_en_distancia UCV</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.001307005127497447</v>
+        <v>0.001515788024780639</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>P.7BE_Está_lejos_en_distancia UCV</t>
+          <t>P. 7N_Están_modernizadasUCAB</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.001095070568942386</v>
+        <v>0.001993824123363014</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>P. 7N_Están_modernizadasUCAB</t>
+          <t>P. 7N_Están_modernizadasUNIMET</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.001762111521870088</v>
+        <v>0.001009623013229578</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>P. 7N_Están_modernizadasUNIMET</t>
+          <t>P.7O_Es_difícil_ser_admitido_e_ingresar UCAB</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.001408138095088619</v>
+        <v>0.001223462903893128</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>P. 7N_Están_modernizadasUSB</t>
+          <t>P.7O_Es_difícil_ser_admitido_e_ingresar USB</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.001362892643541636</v>
+        <v>0.001345895217687142</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>P.7O_Es_difícil_ser_admitido_e_ingresar UCAB</t>
+          <t>P.7O_Es_difícil_ser_admitido_e_ingresar UCV</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.001182331993251903</v>
+        <v>0.001712662787946694</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>P.7O_Es_difícil_ser_admitido_e_ingresar USB</t>
+          <t>P.7S_Ofrecen_ayuda_económica_para_estudiantes_de_pocos_recursos UCAB</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.001624366758423325</v>
+        <v>0.002123504192797087</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>P.7O_Es_difícil_ser_admitido_e_ingresar UCV</t>
+          <t>P.7S_Ofrecen_ayuda_económica_para_estudiantes_de_pocos_recursos UNIMET</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.001775899938619012</v>
+        <v>0.001236180512454609</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>P.7R_Se_puede_pagar_para_obtener_el_título USM</t>
+          <t>P.7S_Ofrecen_ayuda_económica_para_estudiantes_de_pocos_recursos USB</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.000969078725113819</v>
+        <v>0.001531963769476917</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>P.7S_Ofrecen_ayuda_económica_para_estudiantes_de_pocos_recursos UCAB</t>
+          <t>P.7S_Ofrecen_ayuda_económica_para_estudiantes_de_pocos_recursos UCV</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.001977175747828074</v>
+        <v>0.0009911985751503889</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>P.7S_Ofrecen_ayuda_económica_para_estudiantes_de_pocos_recursos UNIMET</t>
+          <t>P.7BC_Tienen_paros _y_conflictos_laborales USB</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.001179818404866902</v>
+        <v>0.0008516271296182056</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>P.7S_Ofrecen_ayuda_económica_para_estudiantes_de_pocos_recursos USB</t>
+          <t>P.7BC_Tienen_paros _y_conflictos_laborales UCV</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.001302902536563989</v>
+        <v>0.001661183067274182</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>P.7S_Ofrecen_ayuda_económica_para_estudiantes_de_pocos_recursos UCV</t>
+          <t>P.7U_Tienen_profesores_honestos UCAB</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.001325162293962284</v>
+        <v>0.001322599858539173</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>P.7BC_Tienen_paros _y_conflictos_laborales USB</t>
+          <t>P.7U_Tienen_profesores_honestos USB</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.00092362900357524</v>
+        <v>0.001157241131433502</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>P.7BC_Tienen_paros _y_conflictos_laborales UCV</t>
+          <t>P.7U_Tienen_profesores_honestos UCV</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.001320387677622688</v>
+        <v>0.001354206707563819</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>P.7U_Tienen_profesores_honestos UCAB</t>
+          <t>P.7BG_Son_de_difícil_acceso UCAB</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.001485735853611466</v>
+        <v>0.001259889606693317</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>P.7U_Tienen_profesores_honestos UNIMET</t>
+          <t>P.7BG_Son_de_difícil_acceso UNIMET</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.00117785499531364</v>
+        <v>0.00113825096151028</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>P.7U_Tienen_profesores_honestos USB</t>
+          <t>P.7BG_Son_de_difícil_acceso USB</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.001050488477363459</v>
+        <v>0.001702944897739704</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>P.7U_Tienen_profesores_honestos UCV</t>
+          <t>P.7BG_Son_de_difícil_acceso UCV</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0.001041095768619052</v>
+        <v>0.001361113399515918</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>P.7BG_Son_de_difícil_acceso UCAB</t>
+          <t>P.7V_Están_comprometidas_con_el_paísUCAB</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.001282828129486897</v>
+        <v>0.00152400847485884</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>P.7BG_Son_de_difícil_acceso UNIMET</t>
+          <t>P.7V_Están_comprometidas_con_el_paísUCV</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>0.001034666769121341</v>
+        <v>0.001281994392760559</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>P.7BG_Son_de_difícil_acceso USB</t>
+          <t>P.7W_Facilitan_conseguir_trabajos_y_empleo_a_sus _egresados UCAB</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>0.001440849916335125</v>
+        <v>0.001688029936188841</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>P.7BG_Son_de_difícil_acceso UCV</t>
+          <t>P.7W_Facilitan_conseguir_trabajos_y_empleo_a_sus _egresados UNIMET</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>0.001549084236916853</v>
+        <v>0.001045793406215452</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>P.7V_Están_comprometidas_con_el_paísUCAB</t>
+          <t>P.7W_Facilitan_conseguir_trabajos_y_empleo_a_sus _egresados USB</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0.001504705931504513</v>
+        <v>0.001146266601309441</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>P.7V_Están_comprometidas_con_el_paísUSB</t>
+          <t>P.7W_Facilitan_conseguir_trabajos_y_empleo_a_sus _egresados UCV</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>0.00126417404280924</v>
+        <v>0.001571377834342301</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>P.7V_Están_comprometidas_con_el_paísUCV</t>
+          <t>P.7X_Tienen_variedad_de_ideologías_y_formas_de_pensar UCAB</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>0.001263475428323783</v>
+        <v>0.002305320729483118</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>P.7W_Facilitan_conseguir_trabajos_y_empleo_a_sus _egresados UCAB</t>
+          <t>P.7X_Tienen_variedad_de_ideologías_y_formas_de_pensar USM</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0.001581007385428688</v>
+        <v>0.001006904183363324</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>P.7W_Facilitan_conseguir_trabajos_y_empleo_a_sus _egresados USB</t>
+          <t>P.7X_Tienen_variedad_de_ideologías_y_formas_de_pensar UCV</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.001239816827271515</v>
+        <v>0.001215264137919342</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>P.7W_Facilitan_conseguir_trabajos_y_empleo_a_sus _egresados UCV</t>
+          <t>P.7BB_El_trayecto_para_llegar_es_peligroso UCAB</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.001077312668440785</v>
+        <v>0.001329719864558833</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>P.7X_Tienen_variedad_de_ideologías_y_formas_de_pensar UCAB</t>
+          <t>P.7BB_El_trayecto_para_llegar_es_peligroso USB</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.001590268857103752</v>
+        <v>0.001322818474421043</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>P.7X_Tienen_variedad_de_ideologías_y_formas_de_pensar UCV</t>
+          <t>P.7BB_El_trayecto_para_llegar_es_peligroso UCV</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>0.001106144584383899</v>
+        <v>0.001432967095957067</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>P.7BB_El_trayecto_para_llegar_es_peligroso USB</t>
+          <t>P.7Y_Cubren_la_demanda_de_carreras UCAB</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.001092461344912392</v>
+        <v>0.001476129681581895</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>P.7BB_El_trayecto_para_llegar_es_peligroso UCV</t>
+          <t>P.7Y_Cubren_la_demanda_de_carreras UNIMET</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.001340701646526923</v>
+        <v>0.0009712641048301372</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>P.7Y_Cubren_la_demanda_de_carreras UCAB</t>
+          <t>P.7Y_Cubren_la_demanda_de_carreras UCV</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.001536376337015077</v>
+        <v>0.001219809456642866</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>P.7Y_Cubren_la_demanda_de_carreras UCV</t>
+          <t>P.7BF_Sus_instalaciones_son_seguras UCAB</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.001349127946825106</v>
+        <v>0.001795554893112497</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>P.7BF_Sus_instalaciones_son_seguras UCAB</t>
+          <t>P.7BF_Sus_instalaciones_son_seguras UNIMET</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.001392069000903028</v>
+        <v>0.001079519602883407</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>P.7BF_Sus_instalaciones_son_seguras UNIMET</t>
+          <t>P.7BF_Sus_instalaciones_son_seguras USB</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.001133513456164561</v>
+        <v>0.0009964908584598599</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>P.7BF_Sus_instalaciones_son_seguras USB</t>
+          <t>P.7Z_Hace_falta_palancas_o_sobornos_para_ingresar UCV</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.0009706049707493644</v>
+        <v>0.001254559855025695</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>P.7Z_Hace_falta_palancas_o_sobornos_para_ingresar UCV</t>
+          <t>P.7AD_Pierden_clases_por_paros_o_conflictos USB</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.001432565006169134</v>
+        <v>0.001573730002159366</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>P.7AD_Pierden_clases_por_paros_o_conflictos USB</t>
+          <t>P.7AD_Pierden_clases_por_paros_o_conflictos UCV</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.001813185338920422</v>
+        <v>0.002844100227924245</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>P.7AD_Pierden_clases_por_paros_o_conflictos UCV</t>
+          <t>P.7BA_No_se_sabe_cuánto_tiempo_toma_graduarse USB</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0.002747424098368143</v>
+        <v>0.001100302768849988</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>P.7BA_No_se_sabe_cuánto_tiempo_toma_graduarse USB</t>
+          <t>P.7BA_No_se_sabe_cuánto_tiempo_toma_graduarse UCV</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>0.001331097127607592</v>
+        <v>0.001154470268337358</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>P.7BA_No_se_sabe_cuánto_tiempo_toma_graduarse UCV</t>
+          <t>P.7BH_Graduarse_allí_ayuda_a_irse_del_paísUCAB</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.001277544741336662</v>
+        <v>0.001814734700629129</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>P.7BH_Graduarse_allí_ayuda_a_irse_del_paísUCAB</t>
+          <t>P.7BH_Graduarse_allí_ayuda_a_irse_del_paísUCV</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.001751341679127895</v>
+        <v>0.001651224716003352</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>P.7BH_Graduarse_allí_ayuda_a_irse_del_paísUSB</t>
+          <t>P.7BI_Tienen_el_mejor_ambiente_para_estudiar_y_socializar1</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.001138128108294735</v>
+        <v>0.001946331887867501</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>P.7BH_Graduarse_allí_ayuda_a_irse_del_paísUCV</t>
+          <t>P.7BI_Tienen_el_mejor_ambiente_para_estudiar_y_socializar4</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.001508369297619788</v>
+        <v>0.00117955630259264</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>P.7BI_Tienen_el_mejor_ambiente_para_estudiar_y_socializar1</t>
+          <t>P.7BI_Tienen_el_mejor_ambiente_para_estudiar_y_socializar3</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>0.001512792991435383</v>
+        <v>0.0012352191485825</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>P.7BI_Tienen_el_mejor_ambiente_para_estudiar_y_socializar4</t>
+          <t>P.7BI_Tienen_el_mejor_ambiente_para_estudiar_y_socializar2</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>0.001425739084578353</v>
+        <v>0.001429212420168596</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>P.7BI_Tienen_el_mejor_ambiente_para_estudiar_y_socializar3</t>
+          <t>P.7CA_Son_las_mejores_para_PsicologíaUCAB</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.001260040162922168</v>
+        <v>0.00139312353880033</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>P.7BI_Tienen_el_mejor_ambiente_para_estudiar_y_socializar2</t>
+          <t>P.7CA_Son_las_mejores_para_PsicologíaUNIMET</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>0.001243396390211369</v>
+        <v>0.0008429259737487692</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>P.7CA_Son_las_mejores_para_PsicologíaUCAB</t>
+          <t>P.7CA_Son_las_mejores_para_PsicologíaUCV</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0.001917713906675036</v>
+        <v>0.001611882896906636</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>P.7CA_Son_las_mejores_para_PsicologíaUSB</t>
+          <t>P.7BZ_Son_las_mejores_para_DerechoUCAB</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>0.001231067717001841</v>
+        <v>0.001188442978723561</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>P.7CA_Son_las_mejores_para_PsicologíaUCV</t>
+          <t>P.7BZ_Son_las_mejores_para_DerechoUNIMET</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0.001099772463875771</v>
+        <v>0.000801331077363611</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>P.7BZ_Son_las_mejores_para_DerechoUCAB</t>
+          <t>P.7BZ_Son_las_mejores_para_DerechoUCV</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>0.001125290963260598</v>
+        <v>0.001166959420215666</v>
       </c>
     </row>
     <row r="158">
@@ -2012,167 +2012,167 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>0.002608314701546581</v>
+        <v>0.002360599776898834</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>P.7BL_Permite_tener_prácticas_y_experiencias_profesionales_a_sus_estudiantes UCV</t>
+          <t>P.7BL_Permite_tener_prácticas_y_experiencias_profesionales_a_sus_estudiantes USB</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0.001101995210053107</v>
+        <v>0.001082427078822761</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>P.7BM_Los_profesores_facilitan_sus_contactos_para_obtener_empleo UCV</t>
+          <t>P.7BL_Permite_tener_prácticas_y_experiencias_profesionales_a_sus_estudiantes UCV</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.001301979310483177</v>
+        <v>0.001182791069826039</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>P.7BN_Los_egresados_son_muy_buenos_en_sus_áreasUCAB</t>
+          <t>P.7BM_Los_profesores_facilitan_sus_contactos_para_obtener_empleo UCAB</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.002576962116894528</v>
+        <v>0.001528034962718812</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>P.7BN_Los_egresados_son_muy_buenos_en_sus_áreasUNIMET</t>
+          <t>P.7BM_Los_profesores_facilitan_sus_contactos_para_obtener_empleo UCV</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.001755210743490509</v>
+        <v>0.001089709932052104</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>P.7BN_Los_egresados_son_muy_buenos_en_sus_áreasUSB</t>
+          <t>P.7BN_Los_egresados_son_muy_buenos_en_sus_áreasUCAB</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.001007423885973591</v>
+        <v>0.002136794791002072</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>P.7BN_Los_egresados_son_muy_buenos_en_sus_áreasUCV</t>
+          <t>P.7BN_Los_egresados_son_muy_buenos_en_sus_áreasUNIMET</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.001473663659311414</v>
+        <v>0.001449873181357783</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>P.7BO_Son_verdaderos_campus_universitariosUCAB</t>
+          <t>P.7BN_Los_egresados_son_muy_buenos_en_sus_áreasUSB</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>0.001296047832735797</v>
+        <v>0.001520121486049044</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>P.7BO_Son_verdaderos_campus_universitariosUNIMET</t>
+          <t>P.7BN_Los_egresados_son_muy_buenos_en_sus_áreasUCV</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>0.001176082275108064</v>
+        <v>0.001122042495972458</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>P.7BO_Son_verdaderos_campus_universitariosUSB</t>
+          <t>P.7BO_Son_verdaderos_campus_universitariosUCAB</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>0.001287375610500581</v>
+        <v>0.001377090097263223</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>P.7BO_Son_verdaderos_campus_universitariosUCV</t>
+          <t>P.7BO_Son_verdaderos_campus_universitariosUNIMET</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.001343113833424446</v>
+        <v>0.001059081847773726</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>P.7BP_Los_programas_de_estudio_son_actualizados_y_completosUCAB</t>
+          <t>P.7BO_Son_verdaderos_campus_universitariosUSB</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0.00134133352726351</v>
+        <v>0.00167009031113839</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>P.7BP_Los_programas_de_estudio_son_actualizados_y_completosUNIMET</t>
+          <t>P.7BO_Son_verdaderos_campus_universitariosUCV</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0.001012546176143874</v>
+        <v>0.001418163565948714</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>P.7BP_Los_programas_de_estudio_son_actualizados_y_completosUSB</t>
+          <t>P.7BP_Los_programas_de_estudio_son_actualizados_y_completosUCAB</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.001008554737489022</v>
+        <v>0.001479529019502047</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>P.7BP_Los_programas_de_estudio_son_actualizados_y_completosUCV</t>
+          <t>P.7BP_Los_programas_de_estudio_son_actualizados_y_completosUSB</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.001124218596769211</v>
+        <v>0.001201742063240711</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>P.7BQ_Son_muy_buenas_para_las_carreras_humanísticasUCAB</t>
+          <t>P.7BP_Los_programas_de_estudio_son_actualizados_y_completosUCV</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.001228640867598467</v>
+        <v>0.001185084936070609</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>P.7BQ_Son_muy_buenas_para_las_carreras_humanísticasUCV</t>
+          <t>P.7BQ_Son_muy_buenas_para_las_carreras_humanísticasUCAB</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.0009441550264835725</v>
+        <v>0.00131671960920436</v>
       </c>
     </row>
     <row r="175">
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.001240761536593437</v>
+        <v>0.001738274360136636</v>
       </c>
     </row>
     <row r="176">
@@ -2192,7 +2192,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>0.0006684695254522952</v>
+        <v>0.001050927321818503</v>
       </c>
     </row>
     <row r="177">
@@ -2202,17 +2202,17 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0.00119024921226572</v>
+        <v>0.001268360975120046</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>P.7BU_Sus_estudiantes_tienen_fama_de_ser_un_poco_irresponsables_con_los_estudios_un_poco_flojos UCAB</t>
+          <t>P.7BU_Sus_estudiantes_tienen_fama_de_ser_un_poco_irresponsables_con_los_estudios_un_poco_flojos UNIMET</t>
         </is>
       </c>
       <c r="B178" t="n">
-        <v>0.001034902943242608</v>
+        <v>0.00104056161044766</v>
       </c>
     </row>
     <row r="179">
@@ -2222,7 +2222,7 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>0.001215416812957804</v>
+        <v>0.001189445128432352</v>
       </c>
     </row>
     <row r="180">
@@ -2232,7 +2232,7 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>0.005151105058935925</v>
+        <v>0.006266838634725096</v>
       </c>
     </row>
     <row r="181">
@@ -2242,7 +2242,7 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>0.001280802323992008</v>
+        <v>0.001451792597989402</v>
       </c>
     </row>
     <row r="182">
@@ -2252,7 +2252,7 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>0.001445450043889599</v>
+        <v>0.001321306492969828</v>
       </c>
     </row>
     <row r="183">
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>0.00133314065145559</v>
+        <v>0.001286409417750379</v>
       </c>
     </row>
     <row r="184">
@@ -2272,17 +2272,17 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>0.003935282139919288</v>
+        <v>0.003198423570323477</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>P.7BW_Las_he_visitado_alguna_vezUSM</t>
+          <t>P.7BW_Las_he_visitado_alguna_vezUNIMET</t>
         </is>
       </c>
       <c r="B185" t="n">
-        <v>0.001132804823032734</v>
+        <v>0.001331379595808973</v>
       </c>
     </row>
     <row r="186">
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>0.001509936868314643</v>
+        <v>0.001656930230262626</v>
       </c>
     </row>
     <row r="187">
@@ -2302,517 +2302,517 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>0.00127946087924314</v>
+        <v>0.001392860600205218</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>P35A_Son malas para estudiar en línea UCAB</t>
+          <t>P.7CB_¿Qué_universidad_han_dado_charlas_en_tu_colegio UCAB</t>
         </is>
       </c>
       <c r="B188" t="n">
-        <v>0.002449857875455369</v>
+        <v>0.0009832702334926946</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>P.8_¿Conoces_o_has_escuchado_alguna_vez_de_la_UCAB?</t>
+          <t>P23C_Son buenas para estudiar en línea 1UCAB</t>
         </is>
       </c>
       <c r="B189" t="n">
-        <v>0.00487252956440217</v>
+        <v>0.009471914110546894</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_1</t>
+          <t>P.8_¿Conoces_o_has_escuchado_alguna_vez_de_la_UCAB?</t>
         </is>
       </c>
       <c r="B190" t="n">
-        <v>0.002235669770051471</v>
+        <v>0.006610242975453708</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_2</t>
+          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_1</t>
         </is>
       </c>
       <c r="B191" t="n">
-        <v>0.001909489490742129</v>
+        <v>0.002462954119913889</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_3</t>
+          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_2</t>
         </is>
       </c>
       <c r="B192" t="n">
-        <v>0.001403408966146559</v>
+        <v>0.00173100087503006</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_4</t>
+          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_3</t>
         </is>
       </c>
       <c r="B193" t="n">
-        <v>0.001796488669427751</v>
+        <v>0.001545591336627533</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_8</t>
+          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_4</t>
         </is>
       </c>
       <c r="B194" t="n">
-        <v>0.001148387035126761</v>
+        <v>0.001635813550688964</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_10</t>
+          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_8</t>
         </is>
       </c>
       <c r="B195" t="n">
-        <v>0.001392020585748961</v>
+        <v>0.001370898146670024</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_13</t>
+          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_10</t>
         </is>
       </c>
       <c r="B196" t="n">
-        <v>0.001038341631049957</v>
+        <v>0.001199400960886054</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>P.9_¿Recuerdas_haber_visto_o_escuchado_publicidad_de_la_UCAB_en_algún_medio?</t>
+          <t>P.8a_¿Por_cuál_de_estas_formas_conociste_o_escuchaste_por_primera_vez_de_la_UCAB?_16</t>
         </is>
       </c>
       <c r="B197" t="n">
-        <v>0.006013673956305445</v>
+        <v>0.001164717869131299</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>(P.9A)_¿En_cuál?_4</t>
+          <t>P.9_¿Recuerdas_haber_visto_o_escuchado_publicidad_de_la_UCAB_en_algún_medio?</t>
         </is>
       </c>
       <c r="B198" t="n">
-        <v>0.001464626401791186</v>
+        <v>0.006414574093312167</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>(P.9A)_¿En_cuál?_7</t>
+          <t>(P.9A)_¿En_cuál?_4</t>
         </is>
       </c>
       <c r="B199" t="n">
-        <v>0.001363394313088215</v>
+        <v>0.001397261891654375</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>(P.9A)_¿En_cuál?_8</t>
+          <t>(P.9A)_¿En_cuál?_7</t>
         </is>
       </c>
       <c r="B200" t="n">
-        <v>0.001744870140577065</v>
+        <v>0.001301266336299775</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>P.11.1_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Mala_Universidad/Es_una_excelente_universidad</t>
+          <t>(P.9A)_¿En_cuál?_8</t>
         </is>
       </c>
       <c r="B201" t="n">
-        <v>0.02747850907707344</v>
+        <v>0.002555566512342717</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>P.11.43_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Mala_la_carrera _de_administración/buena_para_la_carrera_d_ administración</t>
+          <t>P.11.1_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Mala_Universidad/Es_una_excelente_universidad</t>
         </is>
       </c>
       <c r="B202" t="n">
-        <v>0.002558581923137839</v>
+        <v>0.02808214809668222</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>P.11.2_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Tarifas_económicas/Tarifas_costosas</t>
+          <t>P.11.43_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Mala_la_carrera _de_administración/buena_para_la_carrera_d_ administración</t>
         </is>
       </c>
       <c r="B203" t="n">
-        <v>0.01492683398633031</v>
+        <v>0.003227825629322344</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>P.11.33_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Lejos_en_distancia/Cercano_en_distancia</t>
+          <t>P.11.2_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Tarifas_económicas/Tarifas_costosas</t>
         </is>
       </c>
       <c r="B204" t="n">
-        <v>0.02324910202694377</v>
+        <v>0.007883814745306443</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>P.11.5_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Malas_instalaciones_y_recursos/Muy_buenas_instalaciones_y_recursos</t>
+          <t>P.11.33_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Lejos_en_distancia/Cercano_en_distancia</t>
         </is>
       </c>
       <c r="B205" t="n">
-        <v>0.02026004075959004</v>
+        <v>0.025315392620044</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>P.11.7_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Poco_prestigio/Mucho_prestigio</t>
+          <t>P.11.5_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Malas_instalaciones_y_recursos/Muy_buenas_instalaciones_y_recursos</t>
         </is>
       </c>
       <c r="B206" t="n">
-        <v>0.00648572186097617</v>
+        <v>0.01870043942674103</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>P.11.12_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Pocas_carreras_demandadas/Muchas_carreras_demandadas</t>
+          <t>P.11.7_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Poco_prestigio/Mucho_prestigio</t>
         </is>
       </c>
       <c r="B207" t="n">
-        <v>0.005468334970793056</v>
+        <v>0.007525415862656675</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>P.11.13_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_No_exige_práctica_de_una_religión_a_sus_estudiantes_y_personal/Exige_práctica_de_una_religión_a_sus_estudiantes_y_personal</t>
+          <t>P.11.12_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Pocas_carreras_demandadas/Muchas_carreras_demandadas</t>
         </is>
       </c>
       <c r="B208" t="n">
-        <v>0.006917305541608421</v>
+        <v>0.007885673152452316</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>P.11.44_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Mala_la_carrera_de_comunicación_social/buena_para_la_carrera_de_comunicación_social</t>
+          <t>P.11.13_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_No_exige_práctica_de_una_religión_a_sus_estudiantes_y_personal/Exige_práctica_de_una_religión_a_sus_estudiantes_y_personal</t>
         </is>
       </c>
       <c r="B209" t="n">
-        <v>0.003116920214183902</v>
+        <v>0.006864538414665292</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>P.11.45_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Mala_la_carrera_de_derecho/buena_para_la_carrera_de_derecho</t>
+          <t>P.11.44_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Mala_la_carrera_de_comunicación_social/buena_para_la_carrera_de_comunicación_social</t>
         </is>
       </c>
       <c r="B210" t="n">
-        <v>0.001963244569511539</v>
+        <v>0.003235972142844285</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>P.11.15_Según_lo_que_conoces_o_has_escuchado_de_la_UCABB_No_está_politizada/Está_muy_politizada</t>
+          <t>P.11.45_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Mala_la_carrera_de_derecho/buena_para_la_carrera_de_derecho</t>
         </is>
       </c>
       <c r="B211" t="n">
-        <v>0.004575064068730371</v>
+        <v>0.002646865801760987</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>P.11.3_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Baja_exigencia_académica/Alta_exigencia_académica</t>
+          <t>P.11.15_Según_lo_que_conoces_o_has_escuchado_de_la_UCABB_No_está_politizada/Está_muy_politizada</t>
         </is>
       </c>
       <c r="B212" t="n">
-        <v>0.01887029049783277</v>
+        <v>0.004380351042873641</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>P.11.16_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_No_suelen_haber_sobornos_por_notas_o_títulos/Suelen_haber_sobornos_por_notas_o_títulos</t>
+          <t>P.11.3_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Baja_exigencia_académica/Alta_exigencia_académica</t>
         </is>
       </c>
       <c r="B213" t="n">
-        <v>0.00477952956487068</v>
+        <v>0.02625672296193594</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>P.11.27_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Tiene_poca_seguridad/Tiene_mucha_seguridad</t>
+          <t>P.11.16_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_No_suelen_haber_sobornos_por_notas_o_títulos/Suelen_haber_sobornos_por_notas_o_títulos</t>
         </is>
       </c>
       <c r="B214" t="n">
-        <v>0.02381141763573737</v>
+        <v>0.004275956089327302</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>P.11.19_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Hay_una_sola_ideología_y_forma_de_pensar/Hay_muchas_ideologías_y_formas_de_pensar</t>
+          <t>P.11.27_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Tiene_poca_seguridad/Tiene_mucha_seguridad</t>
         </is>
       </c>
       <c r="B215" t="n">
-        <v>0.004521650142223846</v>
+        <v>0.00781951277191395</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>P.11.28_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Es_de_dificil_acceso_para_llegar/Es_de_fácil_acceso_para_llegar</t>
+          <t>P.11.19_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Hay_una_sola_ideología_y_forma_de_pensar/Hay_muchas_ideologías_y_formas_de_pensar</t>
         </is>
       </c>
       <c r="B216" t="n">
-        <v>0.01368602613643346</v>
+        <v>0.006674303957102219</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>P.11.20_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_No_hay_discriminación_de_clases/Hay_discriminación_de_clases</t>
+          <t>P.11.28_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Es_de_dificil_acceso_para_llegar/Es_de_fácil_acceso_para_llegar</t>
         </is>
       </c>
       <c r="B217" t="n">
-        <v>0.005022010784249556</v>
+        <v>0.005102940471408864</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>P.11.25_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Da_poca_ayuda_económica_a_estudiantes_de_pocos_recursos/Da_mucha_ayuda_económica_a_estudiantes_de_bajos_recursos</t>
+          <t>P.11.20_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_No_hay_discriminación_de_clases/Hay_discriminación_de_clases</t>
         </is>
       </c>
       <c r="B218" t="n">
-        <v>0.006277869642448161</v>
+        <v>0.003917872883484406</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>P.11.31_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Es_incierto_el_tiempo_que_toma_graduarse/Es_seguro_el_tiempo_en_que_tardas_en_graduarte</t>
+          <t>P.11.25_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Da_poca_ayuda_económica_a_estudiantes_de_pocos_recursos/Da_mucha_ayuda_económica_a_estudiantes_de_bajos_recursos</t>
         </is>
       </c>
       <c r="B219" t="n">
-        <v>0.007788841911907136</v>
+        <v>0.00793992966302173</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>P.11.29_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_El_trayecto_para_llegar_es_peligroso/El_trayecto_para_llegar_es_seguro</t>
+          <t>P.11.31_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Es_incierto_el_tiempo_que_toma_graduarse/Es_seguro_el_tiempo_en_que_tardas_en_graduarte</t>
         </is>
       </c>
       <c r="B220" t="n">
-        <v>0.007328051054902367</v>
+        <v>0.00618556576919433</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>P.11.22_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Es_neutral_políticamente/Es_de_oposición_políticamente</t>
+          <t>P.11.29_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_El_trayecto_para_llegar_es_peligroso/El_trayecto_para_llegar_es_seguro</t>
         </is>
       </c>
       <c r="B221" t="n">
-        <v>0.006888896603186057</v>
+        <v>0.00499207745227995</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>P.11.8_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Es_fácil_ingresar_ser_admitido/Es_difícil_ingresar_ser_admitido</t>
+          <t>P.11.22_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Es_neutral_políticamente/Es_de_oposición_políticamente</t>
         </is>
       </c>
       <c r="B222" t="n">
-        <v>0.007314809085074485</v>
+        <v>0.007226355436645152</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>P.11.32_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_No_tiene_paros_ni_conflictos_laborales/Suele_tener_paros_y_conflictos_laborales</t>
+          <t>P.11.8_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Es_fácil_ingresar_ser_admitido/Es_difícil_ingresar_ser_admitido</t>
         </is>
       </c>
       <c r="B223" t="n">
-        <v>0.008202204123574745</v>
+        <v>0.007909211132835135</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>P.11.26_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Sus_títulos_tienen_poca_validez_internacional/Sus_títulos_tiene_mucha_validez internacional</t>
+          <t>P.11.32_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_No_tiene_paros_ni_conflictos_laborales/Suele_tener_paros_y_conflictos_laborales</t>
         </is>
       </c>
       <c r="B224" t="n">
-        <v>0.005063688619692974</v>
+        <v>0.00874835406534219</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>P.11.14_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_No_está_comprometida_con_el país/Está _muy_comprometida_con_el_país</t>
+          <t>P.11.26_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Sus_títulos_tienen_poca_validez_internacional/Sus_títulos_tiene_mucha_validez internacional</t>
         </is>
       </c>
       <c r="B225" t="n">
-        <v>0.007677004756750982</v>
+        <v>0.004973675267924227</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>P.11.30_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Graduarse_allí_no_ayuda_a _irse_del_país/Graduarse_allí_ayuda_a_irse_del_país</t>
+          <t>P.11.14_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_No_está_comprometida_con_el país/Está _muy_comprometida_con_el_país</t>
         </is>
       </c>
       <c r="B226" t="n">
-        <v>0.005032680152899999</v>
+        <v>0.005605128245394068</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>P.11.34_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Ambiente_inadecuado_para estudiar_y_socializar/Ambiente_adecuado_para_estudiar_y_socializar</t>
+          <t>P.11.30_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Graduarse_allí_no_ayuda_a _irse_del_país/Graduarse_allí_ayuda_a_irse_del_país</t>
         </is>
       </c>
       <c r="B227" t="n">
-        <v>0.005026034229167853</v>
+        <v>0.005592114895389359</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>P.11.35_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Sus_egresados_tienen_pocas_oportunidades_laborales/Sus_egresados_tienen_muchas_oportunidades_laborales</t>
+          <t>P.11.34_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Ambiente_inadecuado_para estudiar_y_socializar/Ambiente_adecuado_para_estudiar_y_socializar</t>
         </is>
       </c>
       <c r="B228" t="n">
-        <v>0.004861884672352912</v>
+        <v>0.008610563721182582</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>P.11.36_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Atrasada_tecnológicamente/Modernizada_tecnológicamente</t>
+          <t>P.11.35_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Sus_egresados_tienen_pocas_oportunidades_laborales/Sus_egresados_tienen_muchas_oportunidades_laborales</t>
         </is>
       </c>
       <c r="B229" t="n">
-        <v>0.003972886470463258</v>
+        <v>0.004534275079611893</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>P.11.37_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_No_facilita_experiencias_profesionales/Facilita_experiencia_profesionales</t>
+          <t>P.11.36_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Atrasada_tecnológicamente/Modernizada_tecnológicamente</t>
         </is>
       </c>
       <c r="B230" t="n">
-        <v>0.003280599203815519</v>
+        <v>0.003502673225329121</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>P.11.38_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Egresados_de_nivel_regular/Egresados_de_nivel_alto</t>
+          <t>P.11.37_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_No_facilita_experiencias_profesionales/Facilita_experiencia_profesionales</t>
         </is>
       </c>
       <c r="B231" t="n">
-        <v>0.004305586043943379</v>
+        <v>0.004253449965716603</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>P.11.39_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Programas_de_estudios_atrasados/Programas_de_estudios_actualizados</t>
+          <t>P.11.38_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Egresados_de_nivel_regular/Egresados_de_nivel_alto</t>
         </is>
       </c>
       <c r="B232" t="n">
-        <v>0.008470297272176233</v>
+        <v>0.005063289613870719</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>P.11.40_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Mala_para_las_carreras_humanísticas/Buena_para_las_carreras_humanísticas</t>
+          <t>P.11.39_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Programas_de_estudios_atrasados/Programas_de_estudios_actualizados</t>
         </is>
       </c>
       <c r="B233" t="n">
-        <v>0.007487902045001747</v>
+        <v>0.003794024883237281</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>P.11.41_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Estudiantes_flojos/Estudiantes_aplicados</t>
+          <t>P.11.40_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Mala_para_las_carreras_humanísticas/Buena_para_las_carreras_humanísticas</t>
         </is>
       </c>
       <c r="B234" t="n">
-        <v>0.01051455310884819</v>
+        <v>0.008978499341482118</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>P.11.42_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Malas_paralas ingenierías/Buena para las ingenierías</t>
+          <t>P.11.41_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Estudiantes_flojos/Estudiantes_aplicados</t>
         </is>
       </c>
       <c r="B235" t="n">
-        <v>0.004460282195979663</v>
+        <v>0.01021032949269342</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>P.11.46_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Mala_la_carrera_de_psicología/buena_para_la_carrera_de _psicología</t>
+          <t>P.11.42_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Malas_paralas ingenierías/Buena para las ingenierías</t>
         </is>
       </c>
       <c r="B236" t="n">
-        <v>0.002208558055167795</v>
+        <v>0.005895711803295355</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>P.11A_¿Cuál_de_estos_mecanismos_crees_o_has_escuchado_que_usa_la_UCAB_para_seleccionar_nuevos_ingresos_de_pregrado?</t>
+          <t>P.11.46_Según_lo_que_conoces_o_has_escuchado_de_la_UCAB_Mala_la_carrera_de_psicología/buena_para_la_carrera_de _psicología</t>
         </is>
       </c>
       <c r="B237" t="n">
-        <v>0.002751390227803473</v>
+        <v>0.002171513939256261</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>P.19_¿Cuáles_redes_sociales_de_la_UCAB_sigues?_(Marca_tantas_como_apliquen)_4</t>
+          <t>P.11A_¿Cuál_de_estos_mecanismos_crees_o_has_escuchado_que_usa_la_UCAB_para_seleccionar_nuevos_ingresos_de_pregrado?</t>
         </is>
       </c>
       <c r="B238" t="n">
-        <v>0.001063645673158043</v>
+        <v>0.003432227348341819</v>
       </c>
     </row>
     <row r="239">
@@ -2822,7 +2822,7 @@
         </is>
       </c>
       <c r="B239" t="n">
-        <v>0.01026473255871724</v>
+        <v>0.01010423218322017</v>
       </c>
     </row>
     <row r="240">
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="B240" t="n">
-        <v>0.009539004152566722</v>
+        <v>0.01101317507012392</v>
       </c>
     </row>
     <row r="241">
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="B241" t="n">
-        <v>0.006237319770769462</v>
+        <v>0.00700822972287155</v>
       </c>
     </row>
     <row r="242">
@@ -2852,7 +2852,7 @@
         </is>
       </c>
       <c r="B242" t="n">
-        <v>0.009124748669136486</v>
+        <v>0.008611299286600115</v>
       </c>
     </row>
     <row r="243">
@@ -2862,7 +2862,7 @@
         </is>
       </c>
       <c r="B243" t="n">
-        <v>0.008217278460082286</v>
+        <v>0.008600398333872538</v>
       </c>
     </row>
     <row r="244">
@@ -2872,7 +2872,7 @@
         </is>
       </c>
       <c r="B244" t="n">
-        <v>0.02169348698635734</v>
+        <v>0.02019545920823581</v>
       </c>
     </row>
     <row r="245">
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="B245" t="n">
-        <v>0.002032590521678705</v>
+        <v>0.001732505788730518</v>
       </c>
     </row>
     <row r="246">
@@ -2892,7 +2892,7 @@
         </is>
       </c>
       <c r="B246" t="n">
-        <v>0.001364520361367086</v>
+        <v>0.001598758912702358</v>
       </c>
     </row>
     <row r="247">
@@ -2902,7 +2902,7 @@
         </is>
       </c>
       <c r="B247" t="n">
-        <v>0.001665098288011143</v>
+        <v>0.001364034322197486</v>
       </c>
     </row>
     <row r="248">
@@ -2912,7 +2912,7 @@
         </is>
       </c>
       <c r="B248" t="n">
-        <v>0.007380303947274228</v>
+        <v>0.008019203850514876</v>
       </c>
     </row>
     <row r="249">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="B249" t="n">
-        <v>0.02059643097035582</v>
+        <v>0.02333072952339436</v>
       </c>
     </row>
     <row r="250">
@@ -2932,7 +2932,7 @@
         </is>
       </c>
       <c r="B250" t="n">
-        <v>0.00269932583801868</v>
+        <v>0.002370808073341559</v>
       </c>
     </row>
     <row r="251">
@@ -2942,7 +2942,7 @@
         </is>
       </c>
       <c r="B251" t="n">
-        <v>0.001336625256740478</v>
+        <v>0.001480944919911067</v>
       </c>
     </row>
     <row r="252">
@@ -2952,7 +2952,7 @@
         </is>
       </c>
       <c r="B252" t="n">
-        <v>0.001153566841849401</v>
+        <v>0.00103047597920855</v>
       </c>
     </row>
     <row r="253">
@@ -2962,7 +2962,7 @@
         </is>
       </c>
       <c r="B253" t="n">
-        <v>0.001108290873576403</v>
+        <v>0.001220546025936151</v>
       </c>
     </row>
     <row r="254">
@@ -2972,7 +2972,7 @@
         </is>
       </c>
       <c r="B254" t="n">
-        <v>0.001485230950305329</v>
+        <v>0.001236725343872776</v>
       </c>
     </row>
     <row r="255">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="B255" t="n">
-        <v>0.001905633862025329</v>
+        <v>0.001615886901499714</v>
       </c>
     </row>
     <row r="256">
@@ -2992,7 +2992,7 @@
         </is>
       </c>
       <c r="B256" t="n">
-        <v>0.001797181847307191</v>
+        <v>0.001512213388220009</v>
       </c>
     </row>
     <row r="257">
@@ -3002,7 +3002,7 @@
         </is>
       </c>
       <c r="B257" t="n">
-        <v>0.001595879437342527</v>
+        <v>0.001568476191008381</v>
       </c>
     </row>
     <row r="258">
@@ -3012,7 +3012,7 @@
         </is>
       </c>
       <c r="B258" t="n">
-        <v>0.001232798765919134</v>
+        <v>0.001426166695435003</v>
       </c>
     </row>
     <row r="259">
@@ -3022,7 +3022,7 @@
         </is>
       </c>
       <c r="B259" t="n">
-        <v>0.001519852109806404</v>
+        <v>0.001383199869568282</v>
       </c>
     </row>
     <row r="260">
@@ -3032,7 +3032,7 @@
         </is>
       </c>
       <c r="B260" t="n">
-        <v>0.002153963351337367</v>
+        <v>0.002179393543577586</v>
       </c>
     </row>
     <row r="261">
@@ -3042,7 +3042,7 @@
         </is>
       </c>
       <c r="B261" t="n">
-        <v>0.001736382322740054</v>
+        <v>0.001474189873798819</v>
       </c>
     </row>
     <row r="262">
@@ -3052,7 +3052,7 @@
         </is>
       </c>
       <c r="B262" t="n">
-        <v>0.004263914316854976</v>
+        <v>0.003294381624461367</v>
       </c>
     </row>
     <row r="263">
@@ -3062,7 +3062,7 @@
         </is>
       </c>
       <c r="B263" t="n">
-        <v>0.003026285352756119</v>
+        <v>0.002738397488353339</v>
       </c>
     </row>
     <row r="264">
@@ -3072,7 +3072,7 @@
         </is>
       </c>
       <c r="B264" t="n">
-        <v>0.00443128114654306</v>
+        <v>0.00331785838855613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>